<commit_message>
Se realizaron las concluciones y se agregaron las tables de tasas y razones
</commit_message>
<xml_diff>
--- a/Data/pob_estandar.xlsx
+++ b/Data/pob_estandar.xlsx
@@ -11,9 +11,6 @@
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -354,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -376,6 +373,16 @@
           <t>GRUPEDAD_num</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>tasa_arg</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>tasa_ba</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -389,6 +396,12 @@
       <c r="C2">
         <v>1</v>
       </c>
+      <c r="D2">
+        <v>0.5945785478608125</v>
+      </c>
+      <c r="E2">
+        <v>0.3064500065120627</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -402,6 +415,12 @@
       <c r="C3">
         <v>2</v>
       </c>
+      <c r="D3">
+        <v>1.445705271667396</v>
+      </c>
+      <c r="E3">
+        <v>0.9672175163865991</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -415,6 +434,12 @@
       <c r="C4">
         <v>3</v>
       </c>
+      <c r="D4">
+        <v>5.819300470487137</v>
+      </c>
+      <c r="E4">
+        <v>3.356069643118103</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -428,6 +453,12 @@
       <c r="C5">
         <v>4</v>
       </c>
+      <c r="D5">
+        <v>13.6300756774351</v>
+      </c>
+      <c r="E5">
+        <v>8.967211594604592</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -441,6 +472,12 @@
       <c r="C6">
         <v>5</v>
       </c>
+      <c r="D6">
+        <v>25.3488719751971</v>
+      </c>
+      <c r="E6">
+        <v>15.57489373621941</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -454,6 +491,12 @@
       <c r="C7">
         <v>6</v>
       </c>
+      <c r="D7">
+        <v>41.0069980545753</v>
+      </c>
+      <c r="E7">
+        <v>27.23398596874357</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -467,6 +510,12 @@
       <c r="C8">
         <v>7</v>
       </c>
+      <c r="D8">
+        <v>61.65185405828525</v>
+      </c>
+      <c r="E8">
+        <v>40.25066245881963</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -480,6 +529,12 @@
       <c r="C9">
         <v>8</v>
       </c>
+      <c r="D9">
+        <v>90.76379571558829</v>
+      </c>
+      <c r="E9">
+        <v>60.31132462440123</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -493,6 +548,12 @@
       <c r="C10">
         <v>9</v>
       </c>
+      <c r="D10">
+        <v>117.1608152687237</v>
+      </c>
+      <c r="E10">
+        <v>80.90503312049793</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -505,6 +566,12 @@
       </c>
       <c r="C11">
         <v>10</v>
+      </c>
+      <c r="D11">
+        <v>181.4719969299573</v>
+      </c>
+      <c r="E11">
+        <v>128.1804306269727</v>
       </c>
     </row>
   </sheetData>

</xml_diff>